<commit_message>
Adding New Customer Creation Testcase
</commit_message>
<xml_diff>
--- a/com.guru99BankingApp/Config/Gurubanking.xlsx
+++ b/com.guru99BankingApp/Config/Gurubanking.xlsx
@@ -13,6 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Registration" sheetId="2" r:id="rId2"/>
+    <sheet name="Fixed income" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Username</t>
   </si>
@@ -35,9 +37,6 @@
     <t>mngr193675</t>
   </si>
   <si>
-    <t>ysagEje</t>
-  </si>
-  <si>
     <t>ysagEje1</t>
   </si>
   <si>
@@ -51,19 +50,152 @@
   </si>
   <si>
     <t>mngr193678</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Postal code</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>State / Province</t>
+  </si>
+  <si>
+    <t>mary</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>marysmith@doxna.com</t>
+  </si>
+  <si>
+    <t>13 Cedars Road</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Straford</t>
+  </si>
+  <si>
+    <t>london</t>
+  </si>
+  <si>
+    <t>E15 4NE</t>
+  </si>
+  <si>
+    <t>marysmith2019</t>
+  </si>
+  <si>
+    <t>19Mary89</t>
+  </si>
+  <si>
+    <t>NIGERIA</t>
+  </si>
+  <si>
+    <t>invest Today</t>
+  </si>
+  <si>
+    <t>Investment Period</t>
+  </si>
+  <si>
+    <t>Invest Every Month Starting Today</t>
+  </si>
+  <si>
+    <t>Invest Rate</t>
+  </si>
+  <si>
+    <t>Interest Frequency</t>
+  </si>
+  <si>
+    <t>Tax Rate</t>
+  </si>
+  <si>
+    <t>Monthly Compounding</t>
+  </si>
+  <si>
+    <t>Amount after investment period</t>
+  </si>
+  <si>
+    <t>Quarterly Compounding</t>
+  </si>
+  <si>
+    <t>Half yearly Compounding</t>
+  </si>
+  <si>
+    <t>Yearly Compounding</t>
+  </si>
+  <si>
+    <t>ymYputa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mngr199526 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Calibri "/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,7 +206,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -82,14 +214,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFDEDEDE"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -371,16 +520,16 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -388,39 +537,285 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>57985454545</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="28.5">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75">
+      <c r="A2">
+        <v>250</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4">
+        <v>56841.51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75">
+      <c r="A3">
+        <v>500</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4">
+        <v>29735.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75">
+      <c r="A4">
+        <v>300</v>
+      </c>
+      <c r="B4">
+        <v>140</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <v>39241.730000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75">
+      <c r="A5">
+        <v>150</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="4">
+        <v>13778.87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>